<commit_message>
Commit Upto Sales Person
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/testdata/FrontAccounting_XLFile.xlsx
+++ b/src/main/java/com/test/testdata/FrontAccounting_XLFile.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4515" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4515" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LogibData" sheetId="1" r:id="rId1"/>
     <sheet name="SalesTypes" sheetId="2" r:id="rId2"/>
+    <sheet name="SalesPersonData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>username</t>
   </si>
@@ -51,29 +52,55 @@
     <t>Calculation Factor</t>
   </si>
   <si>
-    <t>Retail</t>
-  </si>
-  <si>
-    <t>B2C</t>
-  </si>
-  <si>
-    <t>BGDAD</t>
-  </si>
-  <si>
     <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>C@B</t>
+  </si>
+  <si>
+    <t>B6525D</t>
+  </si>
+  <si>
+    <t>Sales person name</t>
+  </si>
+  <si>
+    <t>Provision</t>
+  </si>
+  <si>
+    <t>Chetan</t>
+  </si>
+  <si>
+    <t>Rahul</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -99,10 +126,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -110,8 +138,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -439,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,15 +497,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1">
-        <v>1.3</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
+      <c r="A3" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>6.5</v>
@@ -475,10 +513,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>5.6</v>
+        <v>56565</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -486,10 +524,57 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>